<commit_message>
Added something that does somehitng but not really working as intended
</commit_message>
<xml_diff>
--- a/Steelmeet/Steelmeet/Testxlsx/SSF-protokoll - Copy.xlsx
+++ b/Steelmeet/Steelmeet/Testxlsx/SSF-protokoll - Copy.xlsx
@@ -363,7 +363,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
-  <x:fonts count="2">
+  <x:fonts count="4">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
@@ -379,13 +379,31 @@
       <x:family val="2"/>
       <x:scheme val="minor"/>
     </x:font>
+    <x:font>
+      <x:strike/>
+    </x:font>
+    <x:font>
+      <x:strike/>
+      <x:color theme="1"/>
+      <x:family val="2"/>
+    </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="4">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF228B22"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFF0000"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="6">
@@ -461,7 +479,7 @@
   <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
-  <x:cellXfs count="8">
+  <x:cellXfs count="21">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -472,6 +490,19 @@
       <x:alignment vertical="top" wrapText="1"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,7 +886,7 @@
   <x:sheetPr>
     <x:pageSetUpPr fitToPage="1"/>
   </x:sheetPr>
-  <x:dimension ref="B3:V53"/>
+  <x:dimension ref="B3:V3716"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
       <x:selection activeCell="J12" sqref="J12"/>
@@ -863,11 +894,11 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <x:col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <x:col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="10.140625" customWidth="1"/>
+    <x:col min="5" max="5" width="12.140625" customWidth="1"/>
+    <x:col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <x:col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
-    <x:col min="8" max="8" width="9.140625" customWidth="1"/>
+    <x:col min="8" max="8" width="9" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="3">
@@ -1056,22 +1087,22 @@
       <x:c r="G16" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H16" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I16" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J16" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K16" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="L16" s="2">
+      <x:c r="H16" s="9">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I16" s="9">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J16" s="9">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K16" s="9">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="L16" s="9">
         <x:v>482.5</x:v>
       </x:c>
-      <x:c r="M16" s="2">
+      <x:c r="M16" s="11">
         <x:v>0</x:v>
       </x:c>
       <x:c r="N16" s="2">
@@ -1099,7 +1130,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V16" s="2">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="17" ht="15" customHeight="1">
@@ -1121,13 +1152,13 @@
       <x:c r="G17" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H17" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I17" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J17" s="2">
+      <x:c r="H17" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I17" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J17" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K17" s="2">
@@ -1164,7 +1195,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V17" s="2">
-        <x:v>0</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="18" ht="15" customHeight="1">
@@ -1186,16 +1217,16 @@
       <x:c r="G18" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H18" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I18" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J18" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K18" s="2">
+      <x:c r="H18" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I18" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J18" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K18" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="L18" s="2">
@@ -1208,7 +1239,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="O18" s="2">
-        <x:v>0</x:v>
+        <x:v>112.5</x:v>
       </x:c>
       <x:c r="P18" s="2">
         <x:v>0</x:v>
@@ -1223,13 +1254,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="T18" s="2">
-        <x:v>0</x:v>
+        <x:v>112.5</x:v>
       </x:c>
       <x:c r="U18" s="2">
-        <x:v>0</x:v>
+        <x:v>79.19471537619592</x:v>
       </x:c>
       <x:c r="V18" s="2">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="19" ht="15" customHeight="1">
@@ -1251,16 +1282,16 @@
       <x:c r="G19" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H19" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I19" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J19" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K19" s="2">
+      <x:c r="H19" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I19" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J19" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K19" s="19">
         <x:v>0</x:v>
       </x:c>
       <x:c r="L19" s="2">
@@ -1294,7 +1325,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V19" s="2">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="20" ht="15" customHeight="1">
@@ -1316,13 +1347,13 @@
       <x:c r="G20" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H20" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I20" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J20" s="2">
+      <x:c r="H20" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I20" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J20" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K20" s="2">
@@ -1359,7 +1390,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V20" s="2">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="21" ht="15" customHeight="1">
@@ -1381,13 +1412,13 @@
       <x:c r="G21" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H21" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I21" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J21" s="2">
+      <x:c r="H21" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I21" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J21" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K21" s="2">
@@ -1424,7 +1455,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V21" s="2">
-        <x:v>0</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="22" ht="15" customHeight="1">
@@ -1446,13 +1477,13 @@
       <x:c r="G22" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H22" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I22" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J22" s="2">
+      <x:c r="H22" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I22" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J22" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K22" s="2">
@@ -1489,7 +1520,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V22" s="2">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="23" ht="15" customHeight="1">
@@ -1511,16 +1542,16 @@
       <x:c r="G23" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H23" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I23" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J23" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K23" s="2">
+      <x:c r="H23" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I23" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J23" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K23" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="L23" s="2">
@@ -1533,7 +1564,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="O23" s="2">
-        <x:v>0</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="P23" s="2">
         <x:v>0</x:v>
@@ -1548,13 +1579,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="T23" s="2">
-        <x:v>0</x:v>
+        <x:v>305</x:v>
       </x:c>
       <x:c r="U23" s="2">
-        <x:v>0</x:v>
+        <x:v>214.86783592735537</x:v>
       </x:c>
       <x:c r="V23" s="2">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="24" ht="15" customHeight="1">
@@ -1576,16 +1607,16 @@
       <x:c r="G24" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H24" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I24" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J24" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="K24" s="2">
+      <x:c r="H24" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I24" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J24" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K24" s="19">
         <x:v>0</x:v>
       </x:c>
       <x:c r="L24" s="2">
@@ -1619,7 +1650,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V24" s="2">
-        <x:v>0</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="25" ht="15" customHeight="1">
@@ -1641,13 +1672,13 @@
       <x:c r="G25" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H25" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I25" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J25" s="2">
+      <x:c r="H25" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I25" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J25" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K25" s="2">
@@ -1684,7 +1715,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V25" s="2">
-        <x:v>0</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="26" ht="15" customHeight="1">
@@ -1706,13 +1737,13 @@
       <x:c r="G26" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H26" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I26" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J26" s="2">
+      <x:c r="H26" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I26" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J26" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K26" s="2">
@@ -1749,7 +1780,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V26" s="2">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="27" ht="15" customHeight="1">
@@ -1771,13 +1802,13 @@
       <x:c r="G27" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H27" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I27" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J27" s="2">
+      <x:c r="H27" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I27" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J27" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K27" s="2">
@@ -1814,7 +1845,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V27" s="2">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="28" ht="15" customHeight="1">
@@ -1836,13 +1867,13 @@
       <x:c r="G28" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H28" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I28" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J28" s="2">
+      <x:c r="H28" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I28" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J28" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K28" s="2">
@@ -1879,7 +1910,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V28" s="2">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="29" ht="15" customHeight="1">
@@ -1901,13 +1932,13 @@
       <x:c r="G29" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H29" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I29" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J29" s="2">
+      <x:c r="H29" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I29" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J29" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K29" s="2">
@@ -1944,7 +1975,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V29" s="2">
-        <x:v>0</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="30" ht="15" customHeight="1">
@@ -1966,13 +1997,13 @@
       <x:c r="G30" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H30" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I30" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J30" s="2">
+      <x:c r="H30" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I30" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J30" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K30" s="2">
@@ -2009,7 +2040,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V30" s="2">
-        <x:v>0</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="31" ht="15" customHeight="1">
@@ -2031,13 +2062,13 @@
       <x:c r="G31" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H31" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I31" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J31" s="2">
+      <x:c r="H31" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I31" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J31" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K31" s="2">
@@ -2074,7 +2105,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V31" s="2">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="32" ht="15" customHeight="1">
@@ -2096,13 +2127,13 @@
       <x:c r="G32" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H32" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I32" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J32" s="2">
+      <x:c r="H32" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I32" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J32" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K32" s="2">
@@ -2139,7 +2170,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V32" s="2">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="33" ht="15" customHeight="1">
@@ -2161,13 +2192,13 @@
       <x:c r="G33" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H33" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I33" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J33" s="2">
+      <x:c r="H33" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I33" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J33" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K33" s="2">
@@ -2204,7 +2235,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V33" s="2">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="34" ht="15" customHeight="1">
@@ -2226,13 +2257,13 @@
       <x:c r="G34" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H34" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I34" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J34" s="2">
+      <x:c r="H34" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I34" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J34" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K34" s="2">
@@ -2269,7 +2300,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V34" s="2">
-        <x:v>0</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="35" ht="15" customHeight="1">
@@ -2291,13 +2322,13 @@
       <x:c r="G35" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H35" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I35" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J35" s="2">
+      <x:c r="H35" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I35" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J35" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K35" s="2">
@@ -2334,7 +2365,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V35" s="2">
-        <x:v>0</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="36" ht="15" customHeight="1">
@@ -2356,13 +2387,13 @@
       <x:c r="G36" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H36" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I36" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J36" s="2">
+      <x:c r="H36" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I36" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J36" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K36" s="2">
@@ -2399,7 +2430,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V36" s="2">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="37" ht="15" customHeight="1">
@@ -2421,13 +2452,13 @@
       <x:c r="G37" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H37" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I37" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J37" s="2">
+      <x:c r="H37" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I37" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J37" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K37" s="2">
@@ -2464,7 +2495,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V37" s="2">
-        <x:v>0</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="38" ht="15" customHeight="1">
@@ -2486,13 +2517,13 @@
       <x:c r="G38" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H38" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I38" s="2">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J38" s="2">
+      <x:c r="H38" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I38" s="17">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J38" s="17">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K38" s="2">
@@ -2529,7 +2560,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V38" s="2">
-        <x:v>0</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="39">
@@ -2551,13 +2582,13 @@
       <x:c r="G39" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H39">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I39">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J39">
+      <x:c r="H39" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I39" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J39" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K39">
@@ -2594,7 +2625,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V39">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="40">
@@ -2616,13 +2647,13 @@
       <x:c r="G40" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H40">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I40">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J40">
+      <x:c r="H40" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I40" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J40" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K40">
@@ -2659,7 +2690,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V40">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="41" ht="38.25" customHeight="1">
@@ -2681,13 +2712,13 @@
       <x:c r="G41" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H41">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I41">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J41">
+      <x:c r="H41" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I41" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J41" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K41">
@@ -2724,7 +2755,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V41">
-        <x:v>0</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="42">
@@ -2746,13 +2777,13 @@
       <x:c r="G42" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H42">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I42">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J42">
+      <x:c r="H42" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I42" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J42" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K42">
@@ -2789,7 +2820,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V42">
-        <x:v>0</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="43">
@@ -2811,13 +2842,13 @@
       <x:c r="G43" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H43">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I43">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J43">
+      <x:c r="H43" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I43" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J43" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K43">
@@ -2854,7 +2885,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V43">
-        <x:v>0</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="44">
@@ -2876,13 +2907,13 @@
       <x:c r="G44" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H44">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I44">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J44">
+      <x:c r="H44" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I44" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J44" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K44">
@@ -2919,7 +2950,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V44">
-        <x:v>0</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="45" ht="15" customHeight="1">
@@ -2941,13 +2972,13 @@
       <x:c r="G45" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H45">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I45">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J45">
+      <x:c r="H45" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I45" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J45" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K45">
@@ -2984,7 +3015,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V45">
-        <x:v>0</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="46">
@@ -3006,13 +3037,13 @@
       <x:c r="G46" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H46">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I46">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J46">
+      <x:c r="H46" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I46" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J46" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K46">
@@ -3049,7 +3080,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V46">
-        <x:v>0</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="47">
@@ -3071,13 +3102,13 @@
       <x:c r="G47" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H47">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I47">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J47">
+      <x:c r="H47" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I47" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J47" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K47">
@@ -3114,7 +3145,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V47">
-        <x:v>0</x:v>
+        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="48">
@@ -3136,13 +3167,13 @@
       <x:c r="G48" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H48">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I48">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J48">
+      <x:c r="H48" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I48" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J48" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K48">
@@ -3179,7 +3210,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V48">
-        <x:v>0</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="49">
@@ -3201,13 +3232,13 @@
       <x:c r="G49" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H49">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I49">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J49">
+      <x:c r="H49" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I49" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J49" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K49">
@@ -3244,7 +3275,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V49">
-        <x:v>0</x:v>
+        <x:v>17</x:v>
       </x:c>
     </x:row>
     <x:row r="50">
@@ -3266,13 +3297,13 @@
       <x:c r="G50" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H50">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I50">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J50">
+      <x:c r="H50" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I50" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J50" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K50">
@@ -3309,7 +3340,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V50">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="51">
@@ -3331,13 +3362,13 @@
       <x:c r="G51" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H51">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I51">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J51">
+      <x:c r="H51" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I51" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J51" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K51">
@@ -3374,7 +3405,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V51">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="52">
@@ -3396,13 +3427,13 @@
       <x:c r="G52" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H52">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I52">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J52">
+      <x:c r="H52" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I52" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J52" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K52">
@@ -3439,7 +3470,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V52">
-        <x:v>0</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="53">
@@ -3461,13 +3492,13 @@
       <x:c r="G53" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="H53">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="I53">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="J53">
+      <x:c r="H53" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I53" s="20">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J53" s="20">
         <x:v>0</x:v>
       </x:c>
       <x:c r="K53">
@@ -3504,8 +3535,217 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="V53">
-        <x:v>0</x:v>
-      </x:c>
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="116">
+      <x:c r="H116" s="12"/>
+      <x:c r="I116" s="12"/>
+      <x:c r="J116" s="12"/>
+      <x:c r="K116" s="8"/>
+      <x:c r="L116" s="8"/>
+      <x:c r="M116" s="10"/>
+    </x:row>
+    <x:row r="216">
+      <x:c r="H216" s="12"/>
+      <x:c r="I216" s="12"/>
+      <x:c r="J216" s="12"/>
+      <x:c r="K216" s="15"/>
+      <x:c r="L216" s="8"/>
+      <x:c r="M216" s="10"/>
+    </x:row>
+    <x:row r="316">
+      <x:c r="H316" s="12"/>
+      <x:c r="I316" s="12"/>
+      <x:c r="J316" s="12"/>
+      <x:c r="K316" s="15"/>
+      <x:c r="L316" s="8"/>
+      <x:c r="M316" s="10"/>
+    </x:row>
+    <x:row r="416">
+      <x:c r="H416" s="12"/>
+      <x:c r="I416" s="12"/>
+      <x:c r="J416" s="12"/>
+      <x:c r="K416" s="8"/>
+      <x:c r="L416" s="8"/>
+      <x:c r="M416" s="10"/>
+    </x:row>
+    <x:row r="516">
+      <x:c r="H516" s="12"/>
+      <x:c r="I516" s="12"/>
+      <x:c r="J516" s="12"/>
+      <x:c r="K516" s="8"/>
+      <x:c r="L516" s="8"/>
+      <x:c r="M516" s="10"/>
+    </x:row>
+    <x:row r="616">
+      <x:c r="H616" s="12"/>
+      <x:c r="I616" s="12"/>
+      <x:c r="J616" s="12"/>
+      <x:c r="K616" s="8"/>
+      <x:c r="L616" s="8"/>
+      <x:c r="M616" s="10"/>
+    </x:row>
+    <x:row r="716">
+      <x:c r="H716" s="12"/>
+      <x:c r="I716" s="12"/>
+      <x:c r="J716" s="12"/>
+      <x:c r="K716" s="8"/>
+      <x:c r="L716" s="8"/>
+      <x:c r="M716" s="10"/>
+    </x:row>
+    <x:row r="816">
+      <x:c r="H816" s="12"/>
+      <x:c r="I816" s="12"/>
+      <x:c r="J816" s="12"/>
+      <x:c r="K816" s="8"/>
+      <x:c r="L816" s="8"/>
+      <x:c r="M816" s="10"/>
+    </x:row>
+    <x:row r="916">
+      <x:c r="H916" s="12"/>
+      <x:c r="I916" s="12"/>
+      <x:c r="J916" s="12"/>
+    </x:row>
+    <x:row r="1016">
+      <x:c r="H1016" s="12"/>
+      <x:c r="I1016" s="12"/>
+      <x:c r="J1016" s="12"/>
+    </x:row>
+    <x:row r="1116">
+      <x:c r="H1116" s="12"/>
+      <x:c r="I1116" s="12"/>
+      <x:c r="J1116" s="12"/>
+    </x:row>
+    <x:row r="1216">
+      <x:c r="H1216" s="12"/>
+      <x:c r="I1216" s="12"/>
+      <x:c r="J1216" s="12"/>
+    </x:row>
+    <x:row r="1316">
+      <x:c r="H1316" s="12"/>
+      <x:c r="I1316" s="12"/>
+      <x:c r="J1316" s="12"/>
+    </x:row>
+    <x:row r="1416">
+      <x:c r="H1416" s="12"/>
+      <x:c r="I1416" s="12"/>
+      <x:c r="J1416" s="12"/>
+    </x:row>
+    <x:row r="1516">
+      <x:c r="H1516" s="12"/>
+      <x:c r="I1516" s="12"/>
+      <x:c r="J1516" s="12"/>
+    </x:row>
+    <x:row r="1616">
+      <x:c r="H1616" s="12"/>
+      <x:c r="I1616" s="12"/>
+      <x:c r="J1616" s="12"/>
+    </x:row>
+    <x:row r="1716">
+      <x:c r="H1716" s="12"/>
+      <x:c r="I1716" s="12"/>
+      <x:c r="J1716" s="12"/>
+    </x:row>
+    <x:row r="1816">
+      <x:c r="H1816" s="12"/>
+      <x:c r="I1816" s="12"/>
+      <x:c r="J1816" s="12"/>
+    </x:row>
+    <x:row r="1916">
+      <x:c r="H1916" s="12"/>
+      <x:c r="I1916" s="12"/>
+      <x:c r="J1916" s="12"/>
+    </x:row>
+    <x:row r="2016">
+      <x:c r="H2016" s="12"/>
+      <x:c r="I2016" s="12"/>
+      <x:c r="J2016" s="12"/>
+    </x:row>
+    <x:row r="2116">
+      <x:c r="H2116" s="12"/>
+      <x:c r="I2116" s="12"/>
+      <x:c r="J2116" s="12"/>
+    </x:row>
+    <x:row r="2216">
+      <x:c r="H2216" s="12"/>
+      <x:c r="I2216" s="12"/>
+      <x:c r="J2216" s="12"/>
+    </x:row>
+    <x:row r="2316">
+      <x:c r="H2316" s="12"/>
+      <x:c r="I2316" s="12"/>
+      <x:c r="J2316" s="12"/>
+    </x:row>
+    <x:row r="2416">
+      <x:c r="H2416" s="12"/>
+      <x:c r="I2416" s="12"/>
+      <x:c r="J2416" s="12"/>
+    </x:row>
+    <x:row r="2516">
+      <x:c r="H2516" s="12"/>
+      <x:c r="I2516" s="12"/>
+      <x:c r="J2516" s="12"/>
+    </x:row>
+    <x:row r="2616">
+      <x:c r="H2616" s="12"/>
+      <x:c r="I2616" s="12"/>
+      <x:c r="J2616" s="12"/>
+    </x:row>
+    <x:row r="2716">
+      <x:c r="H2716" s="12"/>
+      <x:c r="I2716" s="12"/>
+      <x:c r="J2716" s="12"/>
+    </x:row>
+    <x:row r="2816">
+      <x:c r="H2816" s="12"/>
+      <x:c r="I2816" s="12"/>
+      <x:c r="J2816" s="12"/>
+    </x:row>
+    <x:row r="2916">
+      <x:c r="H2916" s="12"/>
+      <x:c r="I2916" s="12"/>
+      <x:c r="J2916" s="12"/>
+    </x:row>
+    <x:row r="3016">
+      <x:c r="H3016" s="12"/>
+      <x:c r="I3016" s="12"/>
+      <x:c r="J3016" s="12"/>
+    </x:row>
+    <x:row r="3116">
+      <x:c r="H3116" s="12"/>
+      <x:c r="I3116" s="12"/>
+      <x:c r="J3116" s="12"/>
+    </x:row>
+    <x:row r="3216">
+      <x:c r="H3216" s="12"/>
+      <x:c r="I3216" s="12"/>
+      <x:c r="J3216" s="12"/>
+    </x:row>
+    <x:row r="3316">
+      <x:c r="H3316" s="12"/>
+      <x:c r="I3316" s="12"/>
+      <x:c r="J3316" s="12"/>
+    </x:row>
+    <x:row r="3416">
+      <x:c r="H3416" s="12"/>
+      <x:c r="I3416" s="12"/>
+      <x:c r="J3416" s="12"/>
+    </x:row>
+    <x:row r="3516">
+      <x:c r="H3516" s="12"/>
+      <x:c r="I3516" s="12"/>
+      <x:c r="J3516" s="12"/>
+    </x:row>
+    <x:row r="3616">
+      <x:c r="H3616" s="12"/>
+      <x:c r="I3616" s="12"/>
+      <x:c r="J3616" s="12"/>
+    </x:row>
+    <x:row r="3716">
+      <x:c r="H3716" s="12"/>
+      <x:c r="I3716" s="12"/>
+      <x:c r="J3716" s="12"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>